<commit_message>
refactor: add foodIntakeFactorKey unknown pattern test case
</commit_message>
<xml_diff>
--- a/src/tests/food-estimation.test-cases.xlsx
+++ b/src/tests/food-estimation.test-cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayuki/WebstormProjects/JibungotoPlanet-backend/src/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FD9996-21A0-1242-A8E6-4C9C8295C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAB6268-7591-FE45-903D-DC360C5CFD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="13" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
+    <workbookView xWindow="-1360" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="11" xr2:uid="{504EB999-7D82-6E4A-B2A0-71B74C50F3FE}"/>
   </bookViews>
   <sheets>
     <sheet name="answers" sheetId="1" r:id="rId1"/>
@@ -2708,8 +2708,8 @@
   </sheetPr>
   <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView showGridLines="0" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4208,7 +4208,7 @@
         <v>130</v>
       </c>
       <c r="D88" s="23" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E88" s="23" t="s">
         <v>17</v>
@@ -7801,8 +7801,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -7875,7 +7875,7 @@
         <v>121</v>
       </c>
       <c r="D2" s="53">
-        <v>57.681677405213115</v>
+        <v>36.320229539482526</v>
       </c>
       <c r="E2" s="45" t="s">
         <v>132</v>
@@ -7914,7 +7914,7 @@
         <v>121</v>
       </c>
       <c r="D3" s="53">
-        <v>40.374478675766689</v>
+        <v>25.422463406174423</v>
       </c>
       <c r="E3" s="46" t="s">
         <v>132</v>
@@ -7953,7 +7953,7 @@
         <v>121</v>
       </c>
       <c r="D4" s="53">
-        <v>27.118793817743864</v>
+        <v>17.075800507239386</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>132</v>
@@ -7992,7 +7992,7 @@
         <v>98</v>
       </c>
       <c r="D5" s="53">
-        <v>16.897647097028454</v>
+        <v>10.639885122095583</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>132</v>
@@ -8031,7 +8031,7 @@
         <v>98</v>
       </c>
       <c r="D6" s="53">
-        <v>133.97349484074635</v>
+        <v>84.358643918056629</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>132</v>
@@ -8070,7 +8070,7 @@
         <v>98</v>
       </c>
       <c r="D7" s="53">
-        <v>14.853221004183123</v>
+        <v>9.3525781589673063</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>132</v>
@@ -8109,7 +8109,7 @@
         <v>122</v>
       </c>
       <c r="D8" s="53">
-        <v>33.419331464170753</v>
+        <v>21.043039045272852</v>
       </c>
       <c r="E8" s="46" t="s">
         <v>132</v>
@@ -8538,7 +8538,7 @@
         <v>111</v>
       </c>
       <c r="D19" s="53">
-        <v>56.244641471068533</v>
+        <v>35.415375912949486</v>
       </c>
       <c r="E19" s="46" t="s">
         <v>132</v>
@@ -8577,7 +8577,7 @@
         <v>126</v>
       </c>
       <c r="D20" s="53">
-        <v>6.7252337743959494</v>
+        <v>4.2346555332779827</v>
       </c>
       <c r="E20" s="46" t="s">
         <v>132</v>
@@ -8616,7 +8616,7 @@
         <v>126</v>
       </c>
       <c r="D21" s="53">
-        <v>38.178570169923162</v>
+        <v>24.03977301699495</v>
       </c>
       <c r="E21" s="46" t="s">
         <v>132</v>
@@ -8694,7 +8694,7 @@
         <v>126</v>
       </c>
       <c r="D23" s="53">
-        <v>63.701594912840548</v>
+        <v>40.110770930118598</v>
       </c>
       <c r="E23" s="46" t="s">
         <v>132</v>
@@ -10669,8 +10669,8 @@
   </sheetPr>
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>